<commit_message>
add PDF to sem2 HW
</commit_message>
<xml_diff>
--- a/Sem2/Данные для семинара.xlsx
+++ b/Sem2/Данные для семинара.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Задачи на выборку данных" sheetId="1" state="visible" r:id="rId2"/>
@@ -534,8 +534,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2110,7 +2110,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="95" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2126,8 +2126,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I52" activeCellId="0" sqref="I52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K74" activeCellId="0" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4585,7 +4585,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="65" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>